<commit_message>
Frenagem múltipla sendo implementada - leitura do input
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0152979-2133-4A2A-B78F-AE8D2787ADDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008D6452-D3DC-41D0-9BB8-8A6C200473A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5AC4A59C-7540-43B9-B5A1-B957E1B00261}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>-</t>
   </si>
@@ -163,13 +163,10 @@
     <t xml:space="preserve"> θ (MDF)</t>
   </si>
   <si>
-    <t>Variáveis</t>
-  </si>
-  <si>
-    <t>Coeficiente de convecção e fluxo de calor</t>
-  </si>
-  <si>
     <t>Iterações</t>
+  </si>
+  <si>
+    <t>Número de ciclos</t>
   </si>
 </sst>
 </file>
@@ -913,14 +910,21 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="34" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -931,21 +935,48 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -956,40 +987,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="34" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1412,7 +1409,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,163 +1431,163 @@
   <sheetData>
     <row r="1" spans="1:17" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
+      <c r="A2" s="26"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="22" t="s">
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="22"/>
+      <c r="O2" s="40"/>
       <c r="P2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="23" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="23"/>
+      <c r="O3" s="41"/>
       <c r="P3" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="24" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="24"/>
+      <c r="O4" s="42"/>
       <c r="P4" s="17">
         <v>44305</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="28" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="30" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="31"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="28" t="s">
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="28"/>
+      <c r="P6" s="24"/>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="29" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="33" t="s">
+      <c r="F7" s="39"/>
+      <c r="G7" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="34"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="29">
+      <c r="M7" s="44"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="39">
         <v>0</v>
       </c>
-      <c r="P7" s="29"/>
+      <c r="P7" s="39"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="25" t="s">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="25" t="s">
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="26"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="25" t="s">
+      <c r="M9" s="28"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="27"/>
+      <c r="P9" s="29"/>
     </row>
     <row r="10" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>44</v>
@@ -1631,7 +1628,7 @@
       <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="37"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="16" t="s">
         <v>19</v>
       </c>
@@ -1727,6 +1724,16 @@
   </sheetData>
   <sheetProtection formatCells="0"/>
   <mergeCells count="20">
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="G6:K6"/>
     <mergeCell ref="G7:K7"/>
@@ -1737,16 +1744,6 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Planilha de input final
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB5627C-F122-4B5F-BDC1-AF1CEE67AEDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB7C639-1020-4C51-870F-E25A2F747103}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,6 +450,15 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,11 +504,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -509,9 +515,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,24 +872,24 @@
   <sheetData>
     <row r="1" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="22" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="25" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="25"/>
+      <c r="O2" s="28"/>
       <c r="P2" s="6" t="s">
         <v>0</v>
       </c>
@@ -894,22 +897,22 @@
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="26" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="26"/>
+      <c r="O3" s="29"/>
       <c r="P3" s="7" t="s">
         <v>1</v>
       </c>
@@ -917,22 +920,22 @@
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="27" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O4" s="27"/>
+      <c r="O4" s="30"/>
       <c r="P4" s="8">
         <v>44318</v>
       </c>
@@ -959,35 +962,35 @@
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="29" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="30"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="29" t="s">
+      <c r="I6" s="16"/>
+      <c r="J6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="30"/>
-      <c r="L6" s="34" t="s">
+      <c r="K6" s="16"/>
+      <c r="L6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="29" t="s">
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="30"/>
+      <c r="P6" s="16"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1">
         <v>0</v>
@@ -997,34 +1000,34 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="14" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="5">
         <v>0</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28">
+      <c r="H7" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31">
         <f>IF(H7="Unica",1,it/COUNTA(Coefs!B4:B1000))</f>
-        <v>40</v>
-      </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1">
         <v>0.5</v>
@@ -1058,33 +1061,33 @@
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="29" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="29" t="s">
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="33"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="29" t="s">
+      <c r="M9" s="35"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="P9" s="30"/>
+      <c r="P9" s="16"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="2:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1133,7 +1136,7 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1183,21 +1186,21 @@
       <c r="B12" s="5">
         <v>1</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="14">
         <v>0.01</v>
       </c>
-      <c r="D12" s="5">
-        <v>960</v>
+      <c r="D12" s="14">
+        <v>190</v>
       </c>
       <c r="E12" s="5">
         <v>0.5</v>
       </c>
       <c r="F12" s="9">
         <f>G12/3</f>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="G12" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12" s="10">
         <v>109</v>
@@ -1478,11 +1481,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="G9:K9"/>
-    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B2:D4"/>
@@ -1498,8 +1503,6 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12" xr:uid="{32E5F16F-17BA-42D5-98D8-B494C46016A7}">
@@ -1520,7 +1523,7 @@
   <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,264 +1558,234 @@
         <v>0</v>
       </c>
       <c r="C4" s="13">
-        <v>0</v>
+        <v>55593.924142780663</v>
       </c>
       <c r="D4" s="13">
-        <v>35.352208431657324</v>
+        <v>103.69072242054578</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C5" s="13">
-        <v>0</v>
+        <v>55593.924142780663</v>
       </c>
       <c r="D5" s="13">
-        <v>35.352208431657324</v>
+        <v>99.245593159730177</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="12">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="C6" s="13">
-        <v>0</v>
+        <v>52648.891605240999</v>
       </c>
       <c r="D6" s="13">
-        <v>46.5</v>
+        <v>94.751684010574621</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="C7" s="13">
-        <v>0</v>
+        <v>47070.846837448924</v>
       </c>
       <c r="D7" s="13">
-        <v>57.653815160742809</v>
+        <v>90.205517066750673</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="12">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="C8" s="13">
-        <v>0</v>
+        <v>39590.25371634787</v>
       </c>
       <c r="D8" s="13">
-        <v>68.78</v>
+        <v>85.603129757258756</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="C9" s="13">
-        <v>0</v>
+        <v>31201.23731486862</v>
       </c>
       <c r="D9" s="13">
-        <v>79.906390798485234</v>
+        <v>80.939969798461817</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
-        <v>3.5</v>
+        <v>0.6</v>
       </c>
       <c r="C10" s="13">
-        <v>0</v>
+        <v>22936.965587279366</v>
       </c>
       <c r="D10" s="13">
-        <v>90.528172517774365</v>
+        <v>76.210758050250689</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
-        <v>4</v>
+        <v>0.7</v>
       </c>
       <c r="C11" s="13">
-        <v>0</v>
+        <v>15646.588697156145</v>
       </c>
       <c r="D11" s="13">
-        <v>100.85551351592143</v>
+        <v>71.409306166199286</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
-        <v>4.5</v>
+        <v>0.8</v>
       </c>
       <c r="C12" s="13">
-        <v>0</v>
+        <v>9844.5519696540978</v>
       </c>
       <c r="D12" s="13">
-        <v>133.99618478542774</v>
+        <v>66.528268989164118</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
-        <v>5</v>
+        <v>0.9</v>
       </c>
       <c r="C13" s="13">
-        <v>0</v>
+        <v>5672.5096013304492</v>
       </c>
       <c r="D13" s="13">
-        <v>165.12748966091127</v>
+        <v>61.55880003615497</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="C14" s="13">
-        <v>0</v>
+        <v>2968.049888742536</v>
       </c>
       <c r="D14" s="13">
-        <v>194.8887228824029</v>
+        <v>56.490058184993636</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
-        <v>6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C15" s="13">
-        <v>0</v>
+        <v>1395.7551406800651</v>
       </c>
       <c r="D15" s="13">
-        <v>200.44969704509737</v>
+        <v>51.308476666873453</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
-        <v>6.5</v>
+        <v>1.2</v>
       </c>
       <c r="C16" s="13">
-        <v>0</v>
+        <v>582.42907963382163</v>
       </c>
       <c r="D16" s="13">
-        <v>205.9</v>
+        <v>45.996633728045971</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="12">
-        <v>7</v>
+        <v>1.3</v>
       </c>
       <c r="C17" s="13">
-        <v>0</v>
+        <v>212.1859028595569</v>
       </c>
       <c r="D17" s="13">
-        <v>211.35651566001502</v>
+        <v>40.531415013368552</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
-        <v>7.5</v>
+        <v>1.4</v>
       </c>
       <c r="C18" s="13">
-        <v>0</v>
+        <v>66.061534624488729</v>
       </c>
       <c r="D18" s="13">
-        <v>218.7957545112408</v>
+        <v>34.880817907697811</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
-        <v>8</v>
+        <v>1.5</v>
       </c>
       <c r="C19" s="13">
-        <v>5886.3</v>
+        <v>17.067922331721402</v>
       </c>
       <c r="D19" s="13">
-        <v>226.17420656761274</v>
+        <v>28.997878953936123</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="12">
-        <v>8.5</v>
+        <v>1.6</v>
       </c>
       <c r="C20" s="13">
-        <v>5219.3</v>
+        <v>3.505580567712256</v>
       </c>
       <c r="D20" s="13">
-        <v>205.86765610487583</v>
+        <v>22.807595441933696</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
-        <v>9</v>
+        <v>1.7</v>
       </c>
       <c r="C21" s="13">
-        <v>4572.3</v>
+        <v>0.53430656780843089</v>
       </c>
       <c r="D21" s="13">
-        <v>185.0628413539078</v>
+        <v>15.982471848900621</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
-        <v>9.5</v>
+        <v>1.8</v>
       </c>
       <c r="C22" s="13">
-        <v>3921.9</v>
+        <v>5.3132513716005879E-2</v>
       </c>
       <c r="D22" s="13">
-        <v>163.56183290587103</v>
+        <v>9.9872734441134785</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="13">
-        <v>10</v>
-      </c>
-      <c r="C23" s="13">
-        <v>3887.7</v>
-      </c>
-      <c r="D23" s="13">
-        <v>136.69219629067382</v>
-      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="13">
-        <v>10.5</v>
-      </c>
-      <c r="C24" s="13">
-        <v>2916.8</v>
-      </c>
-      <c r="D24" s="13">
-        <v>108.46555905527802</v>
-      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="13">
-        <v>11</v>
-      </c>
-      <c r="C25" s="13">
-        <v>1945.9</v>
-      </c>
-      <c r="D25" s="13">
-        <v>78.304352898796239</v>
-      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="13">
-        <v>11.5</v>
-      </c>
-      <c r="C26" s="13">
-        <v>970.9</v>
-      </c>
-      <c r="D26" s="13">
-        <v>39.152176449398119</v>
-      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="13">
-        <v>12</v>
-      </c>
-      <c r="C27" s="13">
-        <v>0</v>
-      </c>
-      <c r="D27" s="13">
-        <v>0</v>
-      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>